<commit_message>
Cover letter is updated.
</commit_message>
<xml_diff>
--- a/Protection Circuits/TPEL Letter/TPEL-Review.xlsx
+++ b/Protection Circuits/TPEL Letter/TPEL-Review.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews" sheetId="1" r:id="rId1"/>
@@ -1328,10 +1328,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1421,18 +1421,34 @@
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="tr-TR" sz="1400" b="0"/>
+            <a:rPr lang="tr-TR" sz="1400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>DPT</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0"/>
+            <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>s with different voltage levels</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0"/>
-            <a:t>- DPTs with different current ratings</a:t>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>DPTs with different current ratings</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1449,7 +1465,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>Induced voltage waveform for different DPTs</a:t>
@@ -1458,7 +1476,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0"/>
-            <a:t>- An analytical approach or a figure like map</a:t>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>An analytical approach or a figure like map</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1475,7 +1501,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>Discussion of filter design on frequency spectrum plot</a:t>
@@ -1498,7 +1526,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>Importance of SC protection for parallel connected transistors</a:t>
@@ -1507,7 +1537,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0"/>
-            <a:t>- Differences of SC protection for single device and parallel connected device</a:t>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Differences of SC protection for single device and parallel connected device</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1518,7 +1556,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>Performance estimation of other SC protection techniques for parallel connected switches</a:t>
@@ -1547,7 +1587,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>Component selection requirements for SCP mechanism</a:t>
@@ -1556,7 +1598,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0"/>
-            <a:t>- SC tests for different level of voltages and currents</a:t>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>SC tests for different level of voltages and currents</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1579,7 +1629,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>Underlining the effect of SCP technique on power loop inductance</a:t>
@@ -1593,7 +1645,10 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>Analytical approach to inductance (?)</a:t>
@@ -1608,7 +1663,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0"/>
-            <a:t>- A better comparison scheme, figure, table etc. of different type of protection techniques for SC GaN HEMTs</a:t>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>A better comparison scheme, figure, table etc. of different type of protection techniques for SC GaN HEMTs</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1619,7 +1682,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>We might add several studies to our reference list</a:t>
@@ -1642,7 +1707,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>We might add the voltage waveforms</a:t>
@@ -1656,7 +1723,9 @@
           <a:r>
             <a:rPr lang="tr-TR" sz="1400" b="0" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
             <a:t>Short circuit current cannot be shown but we can put simulation waveforms</a:t>
@@ -1949,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" activeCellId="1" sqref="P14 A8:K24"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,644 +2257,644 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
       <c r="K33" s="2"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
       <c r="K34" s="2"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
       <c r="K42" s="2"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
       <c r="K49" s="2"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
       <c r="K50" s="2"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
       <c r="K51" s="2"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
       <c r="K52" s="2"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
       <c r="K53" s="2"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
       <c r="K54" s="2"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
       <c r="K55" s="2"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
       <c r="K56" s="2"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
       <c r="K57" s="2"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -2842,279 +2911,279 @@
       <c r="K58" s="2"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
@@ -3129,136 +3198,136 @@
       <c r="J80" s="2"/>
     </row>
     <row r="81" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="4"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="4"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="3"/>
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
-      <c r="J89" s="3"/>
-      <c r="K89" s="3"/>
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
@@ -3411,121 +3480,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cover letter second version is prepared.
</commit_message>
<xml_diff>
--- a/Protection Circuits/TPEL Letter/TPEL-Review.xlsx
+++ b/Protection Circuits/TPEL Letter/TPEL-Review.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Reviews" sheetId="1" r:id="rId1"/>
@@ -2018,7 +2018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A81" sqref="A81:K90"/>
     </sheetView>
   </sheetViews>

</xml_diff>